<commit_message>
Updated ModelCovSelected to include winter covariates
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolde\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolde\Documents\Git\QRF_extrapolation\model_fit_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA84684-924F-49FE-88AF-C8D58188EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3361EAA1-C3B0-41B2-A9B8-384F5BAC81A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="930" windowWidth="38620" windowHeight="21100" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
     <sheet name="CHaMP_Summer_Steelhead" sheetId="2" r:id="rId2"/>
     <sheet name="CHaMP_Redds_Chinook" sheetId="3" r:id="rId3"/>
     <sheet name="CHaMP_Redds_Steelhead" sheetId="4" r:id="rId4"/>
+    <sheet name="CHaMP_Winter_Chinook" sheetId="5" r:id="rId5"/>
+    <sheet name="CHaMP_Winter_Steelhead" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="95">
   <si>
     <t>QRF2</t>
   </si>
@@ -272,6 +274,57 @@
   </si>
   <si>
     <t xml:space="preserve"> LWVol_WetSlow</t>
+  </si>
+  <si>
+    <t>Dpth_Max</t>
+  </si>
+  <si>
+    <t>FishFishCovAqVegCovSome</t>
+  </si>
+  <si>
+    <t>Ucut_Length</t>
+  </si>
+  <si>
+    <t>70% - "0"</t>
+  </si>
+  <si>
+    <t>Land Classificaiton</t>
+  </si>
+  <si>
+    <t>Discharge_fish</t>
+  </si>
+  <si>
+    <t>DpthResid</t>
+  </si>
+  <si>
+    <t>SubEstCandBldr</t>
+  </si>
+  <si>
+    <t>51% "zero" - use CandBldr</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Missing 30% data</t>
+  </si>
+  <si>
+    <t>LWDens</t>
+  </si>
+  <si>
+    <t>LWCount</t>
+  </si>
+  <si>
+    <t>Does this get collected/calculated with DASH?</t>
+  </si>
+  <si>
+    <t>UcutArea_Pct</t>
+  </si>
+  <si>
+    <t>DpthThlwgExit</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kept C&amp;BLDR to be consistant with winter Chinook</t>
   </si>
 </sst>
 </file>
@@ -626,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7274D39-14C0-44C4-9180-575AD48E3D39}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,6 +1177,11 @@
         <v>52</v>
       </c>
     </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1132,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC467E4-A05E-4334-9488-72C3A98196D7}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1206,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1711,6 +1769,11 @@
       </c>
       <c r="F37" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1720,10 +1783,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439CB954-3096-4DF2-8E00-B80366D26FEF}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1783,10 +1846,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1811,10 +1874,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2225,6 +2288,11 @@
       </c>
       <c r="D33" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2234,10 +2302,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB27700-094B-4F46-B24F-FF60290A0831}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2305,10 +2373,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2319,10 +2387,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2794,6 +2862,851 @@
         <v>1</v>
       </c>
       <c r="D37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249F9EFA-368B-4F2F-9ED0-2ED9DB2DCB33}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D4CC892-CE50-41E0-B875-4857B27D2603}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
One quick correction for ModelCovSelected
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolde\Documents\Git\QRF_extrapolation\model_fit_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3361EAA1-C3B0-41B2-A9B8-384F5BAC81A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9B9ECE-FFDA-4009-8077-18032CF62E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-36640" yWindow="4700" windowWidth="26210" windowHeight="14610" firstSheet="2" activeTab="5" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="94">
   <si>
     <t>QRF2</t>
   </si>
@@ -277,9 +277,6 @@
   </si>
   <si>
     <t>Dpth_Max</t>
-  </si>
-  <si>
-    <t>FishFishCovAqVegCovSome</t>
   </si>
   <si>
     <t>Ucut_Length</t>
@@ -2880,7 +2877,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2971,7 +2968,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -2985,7 +2982,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -2999,16 +2996,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3027,7 +3024,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
@@ -3041,7 +3038,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
@@ -3055,7 +3052,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -3086,7 +3083,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -3095,7 +3092,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -3103,7 +3100,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -3117,7 +3114,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -3182,7 +3179,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -3204,7 +3201,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -3232,16 +3229,16 @@
         <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -3263,7 +3260,7 @@
         <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -3277,7 +3274,7 @@
         <v>46</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -3294,10 +3291,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D4CC892-CE50-41E0-B875-4857B27D2603}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D28"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3309,7 +3306,7 @@
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -3326,7 +3323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -3340,7 +3337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3354,7 +3351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3368,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -3382,12 +3379,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -3396,12 +3393,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -3410,12 +3407,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>91</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -3424,12 +3421,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -3438,26 +3435,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -3466,12 +3463,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -3480,26 +3477,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -3508,12 +3505,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -3522,12 +3519,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -3536,12 +3533,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -3550,12 +3547,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -3564,99 +3561,102 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -3664,25 +3664,22 @@
       <c r="D25" s="1">
         <v>0</v>
       </c>
-      <c r="E25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -3693,20 +3690,6 @@
         <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fit QRF models updated script
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolde\Documents\Git\QRF_extrapolation\model_fit_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9B9ECE-FFDA-4009-8077-18032CF62E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223A968C-BF6D-4ABB-94C6-D821BB961142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36640" yWindow="4700" windowWidth="26210" windowHeight="14610" firstSheet="2" activeTab="5" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-36640" yWindow="4700" windowWidth="26210" windowHeight="14610" firstSheet="2" activeTab="4" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="92">
   <si>
     <t>QRF2</t>
   </si>
@@ -288,9 +288,6 @@
     <t>Land Classificaiton</t>
   </si>
   <si>
-    <t>Discharge_fish</t>
-  </si>
-  <si>
     <t>DpthResid</t>
   </si>
   <si>
@@ -312,16 +309,13 @@
     <t>LWCount</t>
   </si>
   <si>
-    <t>Does this get collected/calculated with DASH?</t>
-  </si>
-  <si>
     <t>UcutArea_Pct</t>
   </si>
   <si>
     <t>DpthThlwgExit</t>
   </si>
   <si>
-    <t xml:space="preserve"> Kept C&amp;BLDR to be consistant with winter Chinook</t>
+    <t>Remove to be consistant with other models</t>
   </si>
 </sst>
 </file>
@@ -2301,7 +2295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB27700-094B-4F46-B24F-FF60290A0831}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:B16"/>
     </sheetView>
   </sheetViews>
@@ -2876,8 +2870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249F9EFA-368B-4F2F-9ED0-2ED9DB2DCB33}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2982,7 +2976,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -3002,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>80</v>
@@ -3083,16 +3077,13 @@
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -3100,7 +3091,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -3114,7 +3105,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -3176,10 +3167,10 @@
         <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -3193,7 +3184,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -3201,13 +3192,16 @@
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -3229,16 +3223,16 @@
         <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -3260,7 +3254,7 @@
         <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -3274,13 +3268,13 @@
         <v>46</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3293,16 +3287,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D4CC892-CE50-41E0-B875-4857B27D2603}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -3412,7 +3406,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -3432,7 +3426,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -3482,13 +3476,13 @@
         <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -3510,7 +3504,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -3524,7 +3518,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -3572,7 +3566,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -3600,7 +3594,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -3608,16 +3602,16 @@
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -3639,16 +3633,16 @@
         <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -3670,7 +3664,7 @@
         <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -3684,13 +3678,13 @@
         <v>46</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read in selected covariates from excel file.
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolde\Documents\Git\QRF_extrapolation\model_fit_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223A968C-BF6D-4ABB-94C6-D821BB961142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{867821D9-562B-46BC-9406-4EBE66F4C910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36640" yWindow="4700" windowWidth="26210" windowHeight="14610" firstSheet="2" activeTab="4" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-38510" yWindow="930" windowWidth="38620" windowHeight="21100" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
@@ -672,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7274D39-14C0-44C4-9180-575AD48E3D39}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1776,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439CB954-3096-4DF2-8E00-B80366D26FEF}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2870,7 +2870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249F9EFA-368B-4F2F-9ED0-2ED9DB2DCB33}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cleaned xlsx file and updated cov selection table html
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolde\Documents\Git\QRF_extrapolation\model_fit_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{867821D9-562B-46BC-9406-4EBE66F4C910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8F624B-2C14-4986-8425-CE7226489EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="930" windowWidth="38620" windowHeight="21100" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-34240" yWindow="5200" windowWidth="29320" windowHeight="15090" firstSheet="1" activeTab="5" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="91">
   <si>
     <t>QRF2</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t xml:space="preserve"> LWVol_WetSlow</t>
-  </si>
-  <si>
-    <t>Dpth_Max</t>
   </si>
   <si>
     <t>Ucut_Length</t>
@@ -670,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7274D39-14C0-44C4-9180-575AD48E3D39}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,11 +1165,6 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1181,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC467E4-A05E-4334-9488-72C3A98196D7}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1762,11 +1754,6 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1774,10 +1761,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439CB954-3096-4DF2-8E00-B80366D26FEF}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2281,11 +2268,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2293,10 +2275,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB27700-094B-4F46-B24F-FF60290A0831}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B16"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2854,11 +2836,6 @@
       </c>
       <c r="D37" s="1">
         <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2976,7 +2953,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -2990,16 +2967,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -3018,7 +2995,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
@@ -3032,7 +3009,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
@@ -3046,7 +3023,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>21</v>
@@ -3091,7 +3068,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -3105,7 +3082,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -3170,7 +3147,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -3192,7 +3169,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -3201,7 +3178,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -3223,16 +3200,16 @@
         <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -3254,7 +3231,7 @@
         <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -3268,7 +3245,7 @@
         <v>46</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -3287,7 +3264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D4CC892-CE50-41E0-B875-4857B27D2603}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -3406,7 +3383,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -3420,7 +3397,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -3504,7 +3481,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -3518,7 +3495,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -3602,7 +3579,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -3611,7 +3588,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -3633,16 +3610,16 @@
         <v>39</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -3664,7 +3641,7 @@
         <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -3678,7 +3655,7 @@
         <v>46</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Updated model covariate lists
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -5,20 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolde\Documents\Git\QRF_extrapolation\model_fit_selection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mthoodenvironmental-my.sharepoint.com/personal/mark_roes_mthoodenvironmental_com/Documents/Git/QRF_extrapolation/model_fit_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8F624B-2C14-4986-8425-CE7226489EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{AAA84684-924F-49FE-88AF-C8D58188EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76E65009-7F26-4053-82F6-2A05E1553DD7}"/>
   <bookViews>
-    <workbookView xWindow="-34240" yWindow="5200" windowWidth="29320" windowHeight="15090" firstSheet="1" activeTab="5" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
     <sheet name="CHaMP_Summer_Steelhead" sheetId="2" r:id="rId2"/>
     <sheet name="CHaMP_Redds_Chinook" sheetId="3" r:id="rId3"/>
     <sheet name="CHaMP_Redds_Steelhead" sheetId="4" r:id="rId4"/>
-    <sheet name="CHaMP_Winter_Chinook" sheetId="5" r:id="rId5"/>
-    <sheet name="CHaMP_Winter_Steelhead" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -40,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="77">
   <si>
     <t>QRF2</t>
   </si>
@@ -228,9 +224,6 @@
     <t>If we want to keep CU Freq and remove SlowWater_freq &amp;FastTrub_Freq. High corr with both</t>
   </si>
   <si>
-    <t>Not in Chinook model</t>
-  </si>
-  <si>
     <t xml:space="preserve">highly correlated with LWVol_wet &amp; 0.02 MIC difference. Chose this since it was used in Chinook model. </t>
   </si>
   <si>
@@ -252,9 +245,6 @@
     <t>0.82 corr with LWVol_Wet. 0.03 MIC diff so keeping LWVol_wet</t>
   </si>
   <si>
-    <t>Sin_CL</t>
-  </si>
-  <si>
     <t>Sin_CL not included but needs to be. Not in Chinook</t>
   </si>
   <si>
@@ -276,43 +266,7 @@
     <t xml:space="preserve"> LWVol_WetSlow</t>
   </si>
   <si>
-    <t>Ucut_Length</t>
-  </si>
-  <si>
-    <t>70% - "0"</t>
-  </si>
-  <si>
-    <t>Land Classificaiton</t>
-  </si>
-  <si>
-    <t>DpthResid</t>
-  </si>
-  <si>
-    <t>SubEstCandBldr</t>
-  </si>
-  <si>
-    <t>51% "zero" - use CandBldr</t>
-  </si>
-  <si>
-    <t>Temp</t>
-  </si>
-  <si>
-    <t>Missing 30% data</t>
-  </si>
-  <si>
-    <t>LWDens</t>
-  </si>
-  <si>
-    <t>LWCount</t>
-  </si>
-  <si>
-    <t>UcutArea_Pct</t>
-  </si>
-  <si>
-    <t>DpthThlwgExit</t>
-  </si>
-  <si>
-    <t>Remove to be consistant with other models</t>
+    <t>Sin_CL is duplicate data</t>
   </si>
 </sst>
 </file>
@@ -348,11 +302,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,21 +625,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7274D39-14C0-44C4-9180-575AD48E3D39}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.77734375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -698,7 +656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -712,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -732,7 +690,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -746,7 +704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -760,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -774,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -788,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -802,7 +760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -816,7 +774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -833,7 +791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -847,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -861,10 +819,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -881,7 +839,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -898,7 +856,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -915,7 +873,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -929,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -943,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -960,7 +918,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -977,12 +935,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -991,12 +949,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1005,40 +963,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -1047,72 +1005,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" s="1">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
@@ -1120,12 +1078,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -1134,12 +1092,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
@@ -1148,20 +1106,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1175,20 +1147,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC467E4-A05E-4334-9488-72C3A98196D7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1208,7 +1180,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1233,10 +1205,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1247,10 +1219,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1264,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1278,24 +1250,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1309,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1323,7 +1296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1337,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1351,10 +1324,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1368,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1385,7 +1358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1402,7 +1375,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1419,7 +1392,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1436,7 +1409,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1450,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1467,7 +1440,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1480,11 +1453,8 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1501,7 +1471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1518,7 +1488,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1532,7 +1502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1546,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1560,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -1574,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1588,7 +1558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1602,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -1616,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1630,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -1644,10 +1614,10 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -1664,7 +1634,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -1675,10 +1645,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -1692,7 +1662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -1706,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -1720,10 +1690,10 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -1737,7 +1707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -1764,19 +1734,19 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1796,7 +1766,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1816,7 +1786,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1824,13 +1794,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1844,7 +1814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1852,13 +1822,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1872,12 +1842,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -1885,8 +1855,11 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1900,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1917,7 +1890,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1931,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1945,7 +1918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1962,7 +1935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1976,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1990,7 +1963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -2004,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -2018,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -2032,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -2046,10 +2019,10 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -2063,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -2077,12 +2050,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
@@ -2091,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -2105,10 +2078,10 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -2122,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -2136,7 +2109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -2150,7 +2123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
@@ -2164,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -2178,7 +2151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
@@ -2189,10 +2162,10 @@
         <v>1</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
@@ -2206,7 +2179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -2223,7 +2196,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
@@ -2237,10 +2210,10 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
@@ -2254,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -2277,20 +2250,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB27700-094B-4F46-B24F-FF60290A0831}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2310,7 +2283,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2324,7 +2297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2338,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2346,13 +2319,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2360,13 +2333,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2380,7 +2353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2394,12 +2367,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -2407,8 +2380,11 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2422,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2439,7 +2415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2453,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2467,7 +2443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2481,10 +2457,10 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -2498,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -2512,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -2526,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -2540,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -2554,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2568,10 +2544,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2585,10 +2561,10 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -2605,10 +2581,10 @@
         <v>31</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -2622,7 +2598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -2636,7 +2612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -2650,7 +2626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -2664,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -2678,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -2692,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -2706,7 +2682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -2720,7 +2696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -2734,7 +2710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -2748,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2759,10 +2735,10 @@
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -2776,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -2790,7 +2766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -2804,10 +2780,10 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -2821,10 +2797,10 @@
         <v>0</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -2836,832 +2812,6 @@
       </c>
       <c r="D37" s="1">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249F9EFA-368B-4F2F-9ED0-2ED9DB2DCB33}">
-  <dimension ref="A1:E27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D4CC892-CE50-41E0-B875-4857B27D2603}">
-  <dimension ref="A1:E27"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cov updates, pdp script data loading
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mthoodenvironmental-my.sharepoint.com/personal/mark_roes_mthoodenvironmental_com/Documents/Git/QRF_extrapolation/model_fit_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{AAA84684-924F-49FE-88AF-C8D58188EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76E65009-7F26-4053-82F6-2A05E1553DD7}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{AAA84684-924F-49FE-88AF-C8D58188EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E72A7D0-BDF0-41B0-BAAB-D9B20689A214}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="77">
   <si>
     <t>QRF2</t>
   </si>
@@ -245,9 +245,6 @@
     <t>0.82 corr with LWVol_Wet. 0.03 MIC diff so keeping LWVol_wet</t>
   </si>
   <si>
-    <t>Sin_CL not included but needs to be. Not in Chinook</t>
-  </si>
-  <si>
     <t>Missing 45% data</t>
   </si>
   <si>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>Sin_CL is duplicate data</t>
+  </si>
+  <si>
+    <t>Don't think we want to include this one, it's a 'retired' metric</t>
   </si>
 </sst>
 </file>
@@ -625,21 +625,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7274D39-14C0-44C4-9180-575AD48E3D39}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="15.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -656,7 +656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -670,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -690,7 +690,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -704,7 +704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -718,12 +718,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -732,40 +732,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -774,77 +777,74 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -856,12 +856,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -873,12 +873,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -886,76 +886,79 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="F18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C21" s="1">
         <v>1</v>
       </c>
@@ -963,12 +966,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -977,40 +980,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -1019,72 +1022,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
@@ -1092,12 +1095,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
@@ -1106,12 +1109,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -1120,20 +1123,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1148,19 +1165,19 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="A7:F7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1180,7 +1197,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1236,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1249,8 +1266,11 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1264,11 +1284,11 @@
         <v>1</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1282,7 +1302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1296,7 +1316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1310,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1327,7 +1347,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1341,7 +1361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1358,7 +1378,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1375,7 +1395,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1392,7 +1412,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1409,7 +1429,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1423,7 +1443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1440,7 +1460,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1454,7 +1474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1471,7 +1491,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1488,7 +1508,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1502,7 +1522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1516,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1530,7 +1550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -1544,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1558,7 +1578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1572,7 +1592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -1586,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1600,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -1617,7 +1637,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -1634,7 +1654,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -1648,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -1662,7 +1682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -1676,7 +1696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -1693,7 +1713,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -1707,7 +1727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -1737,16 +1757,16 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1766,7 +1786,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1786,7 +1806,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1800,7 +1820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1814,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1828,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1842,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1856,10 +1876,10 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1873,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1890,7 +1910,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1904,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1918,7 +1938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1935,7 +1955,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1949,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1963,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1977,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1991,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -2005,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -2022,7 +2042,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -2036,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -2050,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -2064,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -2081,7 +2101,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -2095,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -2109,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -2123,7 +2143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
@@ -2137,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -2151,7 +2171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
@@ -2165,7 +2185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
@@ -2179,7 +2199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -2196,7 +2216,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
@@ -2213,7 +2233,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
@@ -2227,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -2250,20 +2270,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB27700-094B-4F46-B24F-FF60290A0831}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2283,7 +2303,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2297,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2311,7 +2331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2325,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2339,7 +2359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2353,7 +2373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2367,7 +2387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2381,10 +2401,10 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2398,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2415,7 +2435,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2429,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2443,7 +2463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2457,10 +2477,10 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -2474,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -2488,7 +2508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -2502,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -2516,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -2530,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2544,10 +2564,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2561,10 +2581,10 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -2581,10 +2601,10 @@
         <v>31</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -2598,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -2612,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -2626,7 +2646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -2640,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -2654,7 +2674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -2668,7 +2688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -2682,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -2696,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -2710,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -2724,7 +2744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2738,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -2752,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -2766,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -2780,10 +2800,10 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -2797,10 +2817,10 @@
         <v>0</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Update covariate selection, consol with winter
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mthoodenvironmental-my.sharepoint.com/personal/mark_roes_mthoodenvironmental_com/Documents/Git/QRF_extrapolation/model_fit_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{AAA84684-924F-49FE-88AF-C8D58188EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E72A7D0-BDF0-41B0-BAAB-D9B20689A214}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{AAA84684-924F-49FE-88AF-C8D58188EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6437D2C3-6EF6-4998-A663-71FC0AD2CE13}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
     <sheet name="CHaMP_Summer_Steelhead" sheetId="2" r:id="rId2"/>
     <sheet name="CHaMP_Redds_Chinook" sheetId="3" r:id="rId3"/>
     <sheet name="CHaMP_Redds_Steelhead" sheetId="4" r:id="rId4"/>
+    <sheet name="CHaMP_Winter_Chinook" sheetId="6" r:id="rId5"/>
+    <sheet name="CHaMP_Winter_Steelhead" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="92">
   <si>
     <t>QRF2</t>
   </si>
@@ -267,6 +269,51 @@
   </si>
   <si>
     <t>Don't think we want to include this one, it's a 'retired' metric</t>
+  </si>
+  <si>
+    <t>UcutArea_Pct</t>
+  </si>
+  <si>
+    <t>Ucut_Length</t>
+  </si>
+  <si>
+    <t>DpthResid</t>
+  </si>
+  <si>
+    <t>DpthThlwgExit</t>
+  </si>
+  <si>
+    <t>SubEstCandBldr</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Missing 30% data</t>
+  </si>
+  <si>
+    <t>LWDens</t>
+  </si>
+  <si>
+    <t>LWCount</t>
+  </si>
+  <si>
+    <t>70% - "0"</t>
+  </si>
+  <si>
+    <t>Not a scaled metric</t>
+  </si>
+  <si>
+    <t>Missing 14% data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51% "zero" </t>
+  </si>
+  <si>
+    <t>Discharge during winter fish survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kept C&amp;BLDR to be consistent with winter Chinook</t>
   </si>
 </sst>
 </file>
@@ -302,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -311,6 +358,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7274D39-14C0-44C4-9180-575AD48E3D39}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,7 +807,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
         <v>76</v>
@@ -1264,7 +1314,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>76</v>
@@ -1754,7 +1804,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1859,7 +1909,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2271,7 +2324,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2370,7 +2423,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -2600,7 +2656,7 @@
       <c r="E21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="4" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2832,6 +2888,877 @@
       </c>
       <c r="D37" s="1">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF70D7E7-EC68-4F41-8E73-DCB784146A9E}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="4"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D4C407-397B-497E-8BBB-B8934DCCDAB1}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="4"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
summer model runs and outputs figs
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mthoodenvironmental-my.sharepoint.com/personal/mark_roes_mthoodenvironmental_com/Documents/Git/QRF_extrapolation/model_fit_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{AAA84684-924F-49FE-88AF-C8D58188EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6437D2C3-6EF6-4998-A663-71FC0AD2CE13}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{AAA84684-924F-49FE-88AF-C8D58188EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF9F6BDA-AD95-4590-84A4-2F3C18EC10AE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7274D39-14C0-44C4-9180-575AD48E3D39}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC467E4-A05E-4334-9488-72C3A98196D7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1698,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="s">
         <v>43</v>
@@ -3340,7 +3340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D4C407-397B-497E-8BBB-B8934DCCDAB1}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
qrf model fit results, first round of covariates.
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{AAA84684-924F-49FE-88AF-C8D58188EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF9F6BDA-AD95-4590-84A4-2F3C18EC10AE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="4" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
@@ -1214,7 +1214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC467E4-A05E-4334-9488-72C3A98196D7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -2899,8 +2899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF70D7E7-EC68-4F41-8E73-DCB784146A9E}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3341,7 +3341,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed Thalweg Exit Depth in habit dict., updated ModelCov.csv, re ran summer chin/stl QRF2_trim
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mthoodenvironmental-my.sharepoint.com/personal/mark_roes_mthoodenvironmental_com/Documents/Git/QRF_extrapolation/model_fit_selection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolde\Documents\Git\QRF_extrapolation\model_fit_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{AAA84684-924F-49FE-88AF-C8D58188EA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65CB0EDB-D146-476B-AAC3-1AEF5D2D4494}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E373F0CA-F76A-4053-86CB-4C165DB1AA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-38310" yWindow="1060" windowWidth="23040" windowHeight="12230" firstSheet="4" activeTab="5" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,10 @@
     <sheet name="CHaMP_Winter_Steelhead" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CHaMP_Redds_Chinook!$A$1:$F$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CHaMP_Redds_Steelhead!$A$1:$F$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CHaMP_Summer_Chinook!$A$1:$F$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CHaMP_Summer_Steelhead!$A$1:$F$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CHaMP_Redds_Chinook!$A$1:$H$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CHaMP_Redds_Steelhead!$A$1:$H$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CHaMP_Summer_Chinook!$A$1:$H$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CHaMP_Summer_Steelhead!$A$1:$H$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="118">
   <si>
     <t>QRF2</t>
   </si>
@@ -304,9 +304,6 @@
     <t>LWCount</t>
   </si>
   <si>
-    <t>70% - "0"</t>
-  </si>
-  <si>
     <t>Not a scaled metric</t>
   </si>
   <si>
@@ -320,6 +317,87 @@
   </si>
   <si>
     <t xml:space="preserve"> Kept C&amp;BLDR to be consistent with winter Chinook</t>
+  </si>
+  <si>
+    <t>QRF3</t>
+  </si>
+  <si>
+    <t>QRF3_sp_comb</t>
+  </si>
+  <si>
+    <t>70% - "0", Not a scaled metric</t>
+  </si>
+  <si>
+    <t>51% - "0", removed</t>
+  </si>
+  <si>
+    <t>56% - "0", removed</t>
+  </si>
+  <si>
+    <t>Removed, pebble count</t>
+  </si>
+  <si>
+    <t>53% - "0". DIDN'T REMOVE</t>
+  </si>
+  <si>
+    <t>71% - "0", removed in trimmed</t>
+  </si>
+  <si>
+    <t>QRF3 comments</t>
+  </si>
+  <si>
+    <t>QRF3 notes</t>
+  </si>
+  <si>
+    <t>removed, pebble count</t>
+  </si>
+  <si>
+    <t>removed, not scaled</t>
+  </si>
+  <si>
+    <t>when in doubt, leave in</t>
+  </si>
+  <si>
+    <t>When in doubt, leave in</t>
+  </si>
+  <si>
+    <t>Removed, no relationship</t>
+  </si>
+  <si>
+    <t>QRF3_notes</t>
+  </si>
+  <si>
+    <t>sp_comb_notes</t>
+  </si>
+  <si>
+    <t>removed, lowest realtive importance by long shot</t>
+  </si>
+  <si>
+    <t>swapped with DpthThlwg_avg</t>
+  </si>
+  <si>
+    <t>added back in</t>
+  </si>
+  <si>
+    <t>added to sp_comb</t>
+  </si>
+  <si>
+    <t>added to be consistant between species</t>
+  </si>
+  <si>
+    <t>when in doubt, leave it in</t>
+  </si>
+  <si>
+    <t>added to match Steelhead</t>
+  </si>
+  <si>
+    <t>Added to match steelhead</t>
+  </si>
+  <si>
+    <t>Sp_comb</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -681,21 +759,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7274D39-14C0-44C4-9180-575AD48E3D39}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="15.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" style="1" customWidth="1"/>
+    <col min="3" max="6" width="15.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -709,10 +789,25 @@
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -725,8 +820,14 @@
       <c r="D2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -739,14 +840,20 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -759,8 +866,14 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -773,8 +886,14 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -787,8 +906,14 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -801,8 +926,17 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -815,11 +949,17 @@
       <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -832,8 +972,14 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -846,8 +992,14 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -860,11 +1012,17 @@
       <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -877,8 +1035,14 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -891,11 +1055,17 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -908,11 +1078,17 @@
       <c r="D14" s="1">
         <v>0</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -925,11 +1101,17 @@
       <c r="D15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -942,11 +1124,17 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -959,8 +1147,14 @@
       <c r="D17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -973,8 +1167,14 @@
       <c r="D18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -987,11 +1187,17 @@
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="F19" t="s">
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1004,44 +1210,69 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21"/>
+      <c r="J21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -1049,41 +1280,65 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -1091,100 +1346,151 @@
       <c r="D26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
@@ -1192,26 +1498,84 @@
       <c r="D33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F34" xr:uid="{D7274D39-14C0-44C4-9180-575AD48E3D39}"/>
+  <autoFilter ref="A1:H36" xr:uid="{D7274D39-14C0-44C4-9180-575AD48E3D39}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1219,11 +1583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC467E4-A05E-4334-9488-72C3A98196D7}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1231,11 +1594,12 @@
     <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1248,14 +1612,23 @@
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1268,8 +1641,14 @@
       <c r="D2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1280,10 +1659,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1294,10 +1679,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1310,8 +1701,14 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1324,11 +1721,17 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -1341,12 +1744,18 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" t="s">
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1359,8 +1768,14 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1373,8 +1788,14 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1387,8 +1808,14 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1401,11 +1828,17 @@
       <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1418,8 +1851,14 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1432,11 +1871,17 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1449,11 +1894,17 @@
       <c r="D14" s="1">
         <v>0</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1466,11 +1917,17 @@
       <c r="D15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -1483,11 +1940,17 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1500,8 +1963,14 @@
       <c r="D17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1514,11 +1983,17 @@
       <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1531,8 +2006,14 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1545,11 +2026,17 @@
       <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="F20" t="s">
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1562,11 +2049,17 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1579,8 +2072,14 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1593,8 +2092,17 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -1607,8 +2115,14 @@
       <c r="D24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -1621,8 +2135,14 @@
       <c r="D25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1635,8 +2155,14 @@
       <c r="D26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1649,8 +2175,14 @@
       <c r="D27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -1663,8 +2195,17 @@
       <c r="D28" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1677,8 +2218,17 @@
       <c r="D29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -1691,11 +2241,17 @@
       <c r="D30" s="1">
         <v>0</v>
       </c>
-      <c r="F30" t="s">
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -1708,11 +2264,17 @@
       <c r="D31" s="1">
         <v>0</v>
       </c>
-      <c r="F31" t="s">
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -1725,8 +2287,17 @@
       <c r="D32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -1739,8 +2310,14 @@
       <c r="D33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -1753,8 +2330,17 @@
       <c r="D34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -1767,11 +2353,17 @@
       <c r="D35" s="1">
         <v>1</v>
       </c>
-      <c r="F35" t="s">
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -1784,8 +2376,17 @@
       <c r="D36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -1798,40 +2399,42 @@
       <c r="D37" s="1">
         <v>0</v>
       </c>
-      <c r="F37" t="s">
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F37" xr:uid="{6EC467E4-A05E-4334-9488-72C3A98196D7}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H37" xr:uid="{6EC467E4-A05E-4334-9488-72C3A98196D7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{439CB954-3096-4DF2-8E00-B80366D26FEF}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" style="1" customWidth="1"/>
+    <col min="4" max="6" width="25.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1845,13 +2448,25 @@
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1864,14 +2479,20 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1879,13 +2500,19 @@
         <v>6</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1898,8 +2525,14 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1907,13 +2540,19 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1926,11 +2565,17 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1943,11 +2588,20 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1960,8 +2614,14 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1974,11 +2634,17 @@
       <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1991,8 +2657,14 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2005,8 +2677,14 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2019,11 +2697,17 @@
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -2036,8 +2720,14 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -2050,8 +2740,14 @@
       <c r="D14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -2064,8 +2760,14 @@
       <c r="D15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -2078,8 +2780,14 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -2092,8 +2800,14 @@
       <c r="D17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -2106,58 +2820,86 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" t="s">
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="J18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="J20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -2165,30 +2907,39 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="F22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -2196,151 +2947,269 @@
       <c r="D24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="1">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1</v>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F33" xr:uid="{439CB954-3096-4DF2-8E00-B80366D26FEF}"/>
+  <autoFilter ref="A1:H35" xr:uid="{439CB954-3096-4DF2-8E00-B80366D26FEF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB27700-094B-4F46-B24F-FF60290A0831}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2348,11 +3217,12 @@
     <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" style="1" customWidth="1"/>
+    <col min="4" max="6" width="20.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2366,13 +3236,25 @@
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2385,8 +3267,14 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -2399,8 +3287,14 @@
       <c r="D3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -2408,13 +3302,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -2422,13 +3322,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2441,11 +3347,17 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2458,8 +3370,17 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2472,11 +3393,17 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2489,8 +3416,14 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2503,11 +3436,17 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2520,8 +3459,14 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2534,8 +3479,14 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2548,11 +3499,17 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -2565,8 +3522,14 @@
       <c r="D14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -2579,8 +3542,14 @@
       <c r="D15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -2593,8 +3562,14 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -2607,8 +3582,14 @@
       <c r="D17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -2621,8 +3602,14 @@
       <c r="D18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2635,11 +3622,17 @@
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2652,11 +3645,17 @@
       <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="F20" t="s">
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -2669,14 +3668,20 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -2689,27 +3694,43 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23"/>
+      <c r="J23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -2717,13 +3738,19 @@
       <c r="D24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -2731,13 +3758,22 @@
       <c r="D25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -2745,13 +3781,22 @@
       <c r="D26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
@@ -2759,13 +3804,19 @@
       <c r="D27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
@@ -2773,83 +3824,131 @@
       <c r="D28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="1">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>105</v>
+      </c>
+      <c r="J32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="1">
-        <v>1</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -2857,67 +3956,117 @@
       <c r="D34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>
       </c>
       <c r="D35" s="1">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-      <c r="D37" s="1">
-        <v>1</v>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F37" xr:uid="{0DB27700-094B-4F46-B24F-FF60290A0831}"/>
+  <autoFilter ref="A1:H38" xr:uid="{0DB27700-094B-4F46-B24F-FF60290A0831}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF70D7E7-EC68-4F41-8E73-DCB784146A9E}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D28"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2926,12 +4075,14 @@
     <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="4"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="22.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -2945,10 +4096,19 @@
         <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H1" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2961,8 +4121,14 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2975,8 +4141,14 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2989,8 +4161,14 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -3003,8 +4181,17 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -3017,8 +4204,17 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -3031,8 +4227,14 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -3045,8 +4247,17 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -3059,8 +4270,17 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -3074,13 +4294,16 @@
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -3093,8 +4316,14 @@
       <c r="D11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -3107,8 +4336,14 @@
       <c r="D12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -3121,8 +4356,14 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -3136,10 +4377,16 @@
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -3152,8 +4399,14 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -3166,8 +4419,14 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -3180,8 +4439,14 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -3194,8 +4459,17 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -3208,8 +4482,14 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -3222,8 +4502,14 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -3236,8 +4522,14 @@
       <c r="D21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -3251,10 +4543,16 @@
         <v>0</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -3267,8 +4565,14 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -3282,10 +4586,16 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
@@ -3299,10 +4609,16 @@
         <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -3315,8 +4631,14 @@
       <c r="D26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -3329,8 +4651,14 @@
       <c r="D27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
@@ -3344,7 +4672,13 @@
         <v>0</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>87</v>
+        <v>117</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3355,10 +4689,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D4C407-397B-497E-8BBB-B8934DCCDAB1}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3366,12 +4700,14 @@
     <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="4"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="5" width="22.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.44140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -3384,11 +4720,20 @@
       <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H1" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -3401,8 +4746,14 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3415,8 +4766,14 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3429,8 +4786,14 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -3443,8 +4806,17 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -3457,8 +4829,17 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -3471,8 +4852,14 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -3485,8 +4872,17 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -3499,8 +4895,17 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -3513,8 +4918,17 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -3527,8 +4941,14 @@
       <c r="D11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -3541,8 +4961,14 @@
       <c r="D12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -3555,8 +4981,14 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -3569,11 +5001,17 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -3586,8 +5024,14 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -3600,8 +5044,14 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -3614,8 +5064,14 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -3628,8 +5084,17 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -3642,8 +5107,14 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -3656,8 +5127,14 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -3670,8 +5147,14 @@
       <c r="D21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -3684,8 +5167,14 @@
       <c r="D22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -3698,11 +5187,17 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -3715,8 +5210,14 @@
       <c r="D24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
@@ -3729,11 +5230,17 @@
       <c r="D25" s="1">
         <v>0</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -3746,8 +5253,14 @@
       <c r="D26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -3760,8 +5273,14 @@
       <c r="D27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
@@ -3774,8 +5293,14 @@
       <c r="D28" s="1">
         <v>0</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>87</v>
+      <c r="E28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional model run outputs
</commit_message>
<xml_diff>
--- a/model_fit_selection/ModelCovSelected.xlsx
+++ b/model_fit_selection/ModelCovSelected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mthoodenvironmental-my.sharepoint.com/personal/mark_roes_mthoodenvironmental_com/Documents/Git/QRF_extrapolation/model_fit_selection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{E373F0CA-F76A-4053-86CB-4C165DB1AA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC15E09D-62E3-4276-824C-2F0846E42945}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{E373F0CA-F76A-4053-86CB-4C165DB1AA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1C52D6E-9BBE-4CB8-83E9-C66FDFEA1D7B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{E5292A8E-66D9-41F1-985A-4E89AADE2F78}"/>
   </bookViews>
   <sheets>
     <sheet name="CHaMP_Summer_Chinook" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="121">
   <si>
     <t>QRF2</t>
   </si>
@@ -5386,10 +5386,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF70D7E7-EC68-4F41-8E73-DCB784146A9E}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5399,13 +5399,13 @@
     <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.44140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="25.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="35.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="8" width="25.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="35.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="23.109375" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -5428,13 +5428,16 @@
         <v>118</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5456,8 +5459,11 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -5479,8 +5485,11 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -5502,8 +5511,11 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -5525,11 +5537,14 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -5551,11 +5566,14 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -5577,8 +5595,11 @@
       <c r="G7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -5600,11 +5621,14 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -5626,11 +5650,14 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -5652,11 +5679,14 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -5678,8 +5708,11 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -5701,8 +5734,11 @@
       <c r="G12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -5724,8 +5760,11 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -5747,11 +5786,14 @@
       <c r="G14" s="1">
         <v>1</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -5773,8 +5815,11 @@
       <c r="G15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -5796,8 +5841,11 @@
       <c r="G16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -5819,8 +5867,11 @@
       <c r="G17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -5842,11 +5893,14 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -5868,8 +5922,11 @@
       <c r="G19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -5891,8 +5948,11 @@
       <c r="G20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -5914,8 +5974,11 @@
       <c r="G21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -5937,11 +6000,14 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -5963,8 +6029,11 @@
       <c r="G23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -5986,11 +6055,14 @@
       <c r="G24" s="1">
         <v>1</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
@@ -6012,11 +6084,14 @@
       <c r="G25" s="1">
         <v>0</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -6038,8 +6113,11 @@
       <c r="G26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -6061,8 +6139,11 @@
       <c r="G27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
@@ -6084,7 +6165,10 @@
       <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -6096,10 +6180,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D4C407-397B-497E-8BBB-B8934DCCDAB1}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6108,13 +6192,13 @@
     <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="1"/>
     <col min="4" max="5" width="22.33203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="25.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.44140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="8" width="25.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="31.44140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="23.109375" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -6136,14 +6220,17 @@
       <c r="G1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -6165,8 +6252,11 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -6188,8 +6278,11 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -6211,8 +6304,11 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -6234,11 +6330,14 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -6260,11 +6359,14 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -6286,8 +6388,11 @@
       <c r="G7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -6309,11 +6414,14 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -6335,11 +6443,14 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -6361,11 +6472,14 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -6387,8 +6501,11 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -6410,8 +6527,11 @@
       <c r="G12" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -6433,8 +6553,11 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -6456,11 +6579,14 @@
       <c r="G14" s="1">
         <v>1</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -6482,8 +6608,11 @@
       <c r="G15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -6505,8 +6634,11 @@
       <c r="G16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -6528,8 +6660,11 @@
       <c r="G17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -6551,11 +6686,14 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -6577,8 +6715,11 @@
       <c r="G19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -6600,8 +6741,11 @@
       <c r="G20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -6623,8 +6767,11 @@
       <c r="G21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -6646,8 +6793,11 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -6669,11 +6819,14 @@
       <c r="G23" s="1">
         <v>1</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -6695,8 +6848,11 @@
       <c r="G24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
@@ -6718,11 +6874,14 @@
       <c r="G25" s="1">
         <v>0</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -6744,8 +6903,11 @@
       <c r="G26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -6767,8 +6929,11 @@
       <c r="G27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
@@ -6790,7 +6955,10 @@
       <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>